<commit_message>
Changed the files according to the needed fix.
</commit_message>
<xml_diff>
--- a/CSE190/Data.xlsx
+++ b/CSE190/Data.xlsx
@@ -62,22 +62,6 @@
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
   <si>
-    <t>~118x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~313x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~181x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
-    <t>~10x</t>
-    <phoneticPr fontId="1" type="noConversion"/>
-  </si>
-  <si>
     <t>Different # of member</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
@@ -91,6 +75,22 @@
   </si>
   <si>
     <t>m = 2000 / f = 50 / p = 10000</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~9.2x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~11.2x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>~4x</t>
+    <phoneticPr fontId="1" type="noConversion"/>
+  </si>
+  <si>
+    <t>8.2x</t>
     <phoneticPr fontId="1" type="noConversion"/>
   </si>
 </sst>
@@ -509,10 +509,10 @@
         <v>77.474431037902804</v>
       </c>
       <c r="H3">
-        <v>1.5690901279449401</v>
+        <v>4.6002864837646401E-2</v>
       </c>
       <c r="I3">
-        <v>6.4063661098480198</v>
+        <v>5.60040473937988E-2</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.3">
@@ -537,7 +537,7 @@
         <v>4.9998760223388602E-3</v>
       </c>
       <c r="I7">
-        <v>5.4003238677978502E-2</v>
+        <v>5.0010681152343698E-3</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.3">
@@ -557,10 +557,10 @@
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H9" t="s">
-        <v>12</v>
+        <v>15</v>
       </c>
       <c r="I9" t="s">
-        <v>11</v>
+        <v>16</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.3">
@@ -611,10 +611,10 @@
         <v>12.5097148418426</v>
       </c>
       <c r="H15">
+        <v>1.6000986099243102E-2</v>
+      </c>
+      <c r="I15">
         <v>4.1002988815307603E-2</v>
-      </c>
-      <c r="I15">
-        <v>1.4490828514099099</v>
       </c>
     </row>
     <row r="18" spans="1:9" x14ac:dyDescent="0.3">
@@ -636,10 +636,10 @@
         <v>3</v>
       </c>
       <c r="H19">
-        <v>4.0001869201660104E-3</v>
+        <v>3.9999485015869097E-3</v>
       </c>
       <c r="I19">
-        <v>8.0008506774902292E-3</v>
+        <v>5.00082969665527E-3</v>
       </c>
     </row>
     <row r="20" spans="1:9" x14ac:dyDescent="0.3">
@@ -659,10 +659,10 @@
     </row>
     <row r="21" spans="1:9" x14ac:dyDescent="0.3">
       <c r="H21" t="s">
-        <v>14</v>
+        <v>17</v>
       </c>
       <c r="I21" t="s">
-        <v>13</v>
+        <v>18</v>
       </c>
     </row>
     <row r="23" spans="1:9" x14ac:dyDescent="0.3">
@@ -695,10 +695,10 @@
     </row>
     <row r="25" spans="1:9" x14ac:dyDescent="0.3">
       <c r="A25" t="s">
-        <v>15</v>
+        <v>11</v>
       </c>
       <c r="B25" t="s">
-        <v>16</v>
+        <v>12</v>
       </c>
       <c r="C25">
         <v>0.180009365081787</v>
@@ -713,15 +713,15 @@
         <v>87.065979957580495</v>
       </c>
       <c r="H25">
-        <v>3.0000209808349601E-3</v>
+        <v>6.0009956359863203E-3</v>
       </c>
       <c r="I25">
-        <v>3.2001018524169901E-2</v>
+        <v>4.9998760223388602E-3</v>
       </c>
     </row>
     <row r="26" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B26" t="s">
-        <v>17</v>
+        <v>13</v>
       </c>
       <c r="C26">
         <v>0.78104615211486805</v>
@@ -736,10 +736,10 @@
         <v>93.924371957778902</v>
       </c>
       <c r="H26">
-        <v>3.9999485015869097E-3</v>
+        <v>5.0010681152343698E-3</v>
       </c>
       <c r="I26">
-        <v>3.9001941680908203E-2</v>
+        <v>5.0001144409179601E-3</v>
       </c>
     </row>
     <row r="27" spans="1:9" x14ac:dyDescent="0.3">
@@ -762,12 +762,12 @@
         <v>4.9998760223388602E-3</v>
       </c>
       <c r="I27">
-        <v>5.4003238677978502E-2</v>
+        <v>5.0010681152343698E-3</v>
       </c>
     </row>
     <row r="28" spans="1:9" x14ac:dyDescent="0.3">
       <c r="B28" t="s">
-        <v>18</v>
+        <v>14</v>
       </c>
       <c r="C28">
         <v>4.0672333240508998</v>
@@ -782,10 +782,10 @@
         <v>106.891113996505</v>
       </c>
       <c r="H28">
-        <v>4.0009021759033203E-3</v>
+        <v>6.0009956359863203E-3</v>
       </c>
       <c r="I28">
-        <v>3.6002159118652302E-2</v>
+        <v>6.0000419616699201E-3</v>
       </c>
     </row>
   </sheetData>

</xml_diff>